<commit_message>
#242  - remove 'other' option
</commit_message>
<xml_diff>
--- a/run/output/iecorrect/iecorrect-template-multiple-ids.xlsx
+++ b/run/output/iecorrect/iecorrect-template-multiple-ids.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="19" uniqueCount="8">
   <si>
     <t>make</t>
   </si>
@@ -38,46 +38,13 @@
     <t>notes</t>
   </si>
   <si>
-    <t>make</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>varname</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>valuecurrent</t>
-  </si>
-  <si>
-    <t>initials</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>make</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>n_obs</t>
   </si>
-  <si>
-    <t>initials</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -116,8 +83,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -157,31 +127,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -198,25 +171,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">

</xml_diff>